<commit_message>
Finished analysis of Alt1
</commit_message>
<xml_diff>
--- a/Excel_Challenge_618 - Project Plan with Relationship.xlsx
+++ b/Excel_Challenge_618 - Project Plan with Relationship.xlsx
@@ -8,13 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7C33AB7-C5D3-43F2-99CD-ACE978CF4B67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85C38C82-0A61-4E1C-86EE-4E318DA1ECAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{ADEF83EE-B1CF-4CAF-A2E9-FA4EF76291CB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{ADEF83EE-B1CF-4CAF-A2E9-FA4EF76291CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
+    <sheet name="Alt1" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_a">'Alt1'!$G$18:$G$27</definedName>
+    <definedName name="_b">'Alt1'!$H$18:$H$27</definedName>
+    <definedName name="_dur">'Alt1'!$D$3:$D$12</definedName>
+    <definedName name="_pfull">'Alt1'!$F$18:$F$27</definedName>
+    <definedName name="_std">'Alt1'!$B$3</definedName>
+    <definedName name="_task">'Alt1'!$A$3:$A$12</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,8 +44,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="20">
   <si>
     <t>Answer Expected</t>
   </si>
@@ -87,6 +118,15 @@
   </si>
   <si>
     <t>https://www.linkedin.com/feed/update/urn:li:activity:7278258300758937600/</t>
+  </si>
+  <si>
+    <t>PredFull</t>
+  </si>
+  <si>
+    <t>Finish</t>
+  </si>
+  <si>
+    <t>Great use of SCAN</t>
   </si>
 </sst>
 </file>
@@ -110,7 +150,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -129,6 +169,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -142,7 +188,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -155,6 +201,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -178,14 +225,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>30480</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>102870</xdr:rowOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>80010</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>443230</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>34290</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -200,8 +247,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="30480" y="1760220"/>
-          <a:ext cx="3771900" cy="2164080"/>
+          <a:off x="30480" y="2457450"/>
+          <a:ext cx="3719830" cy="2148840"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -439,6 +486,55 @@
             <a:schemeClr val="tx1"/>
           </a:solidFill>
         </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>510540</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>578160</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>42248</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4" descr="A computer code with text&#10;&#10;AI-generated content may be incorrect.">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12172168-2964-C215-3344-C60B108F1A77}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6332220" y="0"/>
+          <a:ext cx="6773220" cy="2419688"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -761,13 +857,42 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="649" row="8">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{6528BAAC-9ECB-48D7-B8A5-2986890A82FF}">
+  <we:reference id="wa200003696" version="1.3.0.0" store="en-US" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="wa200003696" version="1.3.0.0" store="" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties>
+    <we:property name="projectV0_1-56c6e055-265e-4713-816e-a646dbb708de" value="{&quot;kind&quot;:&quot;AFEJSONBlobNode&quot;,&quot;id&quot;:&quot;{1EF13DA5-5E49-4A3F-B222-FEA447D244EB}&quot;}"/>
+  </we:properties>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+  <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
+      <we:customFunctionIdList>
+        <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
+      </we:customFunctionIdList>
+    </a:ext>
+  </we:extLst>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57537860-8F30-47D9-A8E5-8D6F48BC9AB1}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -994,4 +1119,724 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0568273B-8D1A-45CB-A97A-A6D6AA401640}">
+  <dimension ref="A1:N40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.88671875" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="F1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="1"/>
+      <c r="N1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="4">
+        <v>45627</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>45627</v>
+      </c>
+      <c r="G3" s="4">
+        <v>45627</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="5">
+        <v>4</v>
+      </c>
+      <c r="F4" s="4">
+        <v>45627</v>
+      </c>
+      <c r="G4" s="4">
+        <v>45631</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="5">
+        <v>10</v>
+      </c>
+      <c r="F5" s="4">
+        <v>45631</v>
+      </c>
+      <c r="G5" s="4">
+        <v>45641</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="5">
+        <v>8</v>
+      </c>
+      <c r="F6" s="4">
+        <v>45627</v>
+      </c>
+      <c r="G6" s="4">
+        <v>45635</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="5">
+        <v>3</v>
+      </c>
+      <c r="F7" s="4">
+        <v>45641</v>
+      </c>
+      <c r="G7" s="4">
+        <v>45644</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="5">
+        <v>7</v>
+      </c>
+      <c r="F8" s="4">
+        <v>45631</v>
+      </c>
+      <c r="G8" s="4">
+        <v>45638</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="5">
+        <v>5</v>
+      </c>
+      <c r="F9" s="4">
+        <v>45638</v>
+      </c>
+      <c r="G9" s="4">
+        <v>45643</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="5">
+        <v>10</v>
+      </c>
+      <c r="F10" s="4">
+        <v>45638</v>
+      </c>
+      <c r="G10" s="4">
+        <v>45648</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="5">
+        <v>4</v>
+      </c>
+      <c r="F11" s="4">
+        <v>45648</v>
+      </c>
+      <c r="G11" s="4">
+        <v>45652</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="5">
+        <v>0</v>
+      </c>
+      <c r="F12" s="4">
+        <v>45652</v>
+      </c>
+      <c r="G12" s="4">
+        <v>45652</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="F16" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="F17" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17" t="s">
+        <v>6</v>
+      </c>
+      <c r="J17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B18" t="str" cm="1">
+        <f t="array" ref="B18:C28">_xlfn.LET(_xlpm.hdr, _xlfn.HSTACK("Plan Start", "PLan End"), _xlpm.std, B3, _xlpm._task, A3:A12, _xlpm._pred, C3:C12, _xlpm._dur, D3:D12, _xlpm._predfull, IF(_xlpm._pred = "", "Start", _xlpm._pred), _xlpm._s5, _xlfn.MAP(_xlpm._task, _xlfn.LAMBDA(_xlpm.w, _xlfn.LET(_xlpm.a, _xlfn.SCAN(_xlpm.w, _xlfn.SEQUENCE(ROWS(_xlpm._task)), _xlfn.LAMBDA(_xlpm.x,_xlpm.y, _xlfn.XLOOKUP(_xlpm.x, _xlpm._task, _xlpm._predfull))), _xlpm.b, _xlfn.XLOOKUP(_xlpm.a, _xlpm._task, _xlpm._dur), _xlpm.c, SUM(_xlpm.b) + _xlpm.std, _xlpm.c))), _xlpm._s6, _xlpm._s5 + _xlpm._dur, _xlpm._s7, _xlfn.HSTACK(_xlpm._s5, _xlpm._s6), _xlpm.ans, _xlfn.VSTACK(_xlpm.hdr, _xlpm._s7), _xlpm.ans)</f>
+        <v>Plan Start</v>
+      </c>
+      <c r="C18" t="str">
+        <v>PLan End</v>
+      </c>
+      <c r="D18" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" t="str" cm="1">
+        <f t="array" ref="G18:G27">_xlfn.SCAN(F16,_xlfn.SEQUENCE(ROWS(_task)),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.XLOOKUP(_xlpm.a,_task,_pfull)))</f>
+        <v>Task1</v>
+      </c>
+      <c r="H18" cm="1">
+        <f t="array" ref="H18:H27">_xlfn.XLOOKUP(_a,_task,_dur)</f>
+        <v>4</v>
+      </c>
+      <c r="I18" s="4">
+        <f>SUM(_b)+_std</f>
+        <v>45631</v>
+      </c>
+      <c r="J18" s="4">
+        <f>I18+_xlfn.XLOOKUP(F16,_task,_dur)</f>
+        <v>45638</v>
+      </c>
+      <c r="K18" s="6" t="str">
+        <f>I18&amp;"|"&amp;J18</f>
+        <v>45631|45638</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B19" s="4">
+        <v>45627</v>
+      </c>
+      <c r="C19" s="4">
+        <v>45627</v>
+      </c>
+      <c r="D19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19" t="str">
+        <v>Start</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B20" s="4">
+        <v>45627</v>
+      </c>
+      <c r="C20" s="4">
+        <v>45631</v>
+      </c>
+      <c r="D20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" t="str">
+        <v>Start</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B21" s="4">
+        <v>45631</v>
+      </c>
+      <c r="C21" s="4">
+        <v>45641</v>
+      </c>
+      <c r="D21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" t="s">
+        <v>6</v>
+      </c>
+      <c r="G21" t="str">
+        <v>Start</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B22" s="4">
+        <v>45627</v>
+      </c>
+      <c r="C22" s="4">
+        <v>45635</v>
+      </c>
+      <c r="D22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" t="s">
+        <v>8</v>
+      </c>
+      <c r="G22" t="str">
+        <v>Start</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B23" s="4">
+        <v>45641</v>
+      </c>
+      <c r="C23" s="4">
+        <v>45644</v>
+      </c>
+      <c r="D23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" t="s">
+        <v>7</v>
+      </c>
+      <c r="G23" t="str">
+        <v>Start</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B24" s="4">
+        <v>45631</v>
+      </c>
+      <c r="C24" s="4">
+        <v>45638</v>
+      </c>
+      <c r="D24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" t="str">
+        <v>Start</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B25" s="4">
+        <v>45638</v>
+      </c>
+      <c r="C25" s="4">
+        <v>45643</v>
+      </c>
+      <c r="D25" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" t="str">
+        <v>Start</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B26" s="4">
+        <v>45638</v>
+      </c>
+      <c r="C26" s="4">
+        <v>45648</v>
+      </c>
+      <c r="D26" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" t="str">
+        <v>Start</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B27" s="4">
+        <v>45648</v>
+      </c>
+      <c r="C27" s="4">
+        <v>45652</v>
+      </c>
+      <c r="D27" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" t="str">
+        <v>Start</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B28" s="4">
+        <v>45652</v>
+      </c>
+      <c r="C28" s="4">
+        <v>45652</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B30" s="4"/>
+      <c r="I30" t="str">
+        <f>K18</f>
+        <v>45631|45638</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B31" s="4"/>
+      <c r="H31" t="s">
+        <v>6</v>
+      </c>
+      <c r="I31" t="str">
+        <f t="dataTable" ref="I31:I40" dt2D="0" dtr="0" r1="F16"/>
+        <v>45627|45627</v>
+      </c>
+      <c r="J31" s="4" cm="1">
+        <f t="array" ref="J31:K31">_xlfn.TEXTSPLIT(I31,"|")+0</f>
+        <v>45627</v>
+      </c>
+      <c r="K31" s="4">
+        <v>45627</v>
+      </c>
+      <c r="M31" t="b" cm="1">
+        <f t="array" ref="M31:N40">J31:K40=F3:G12</f>
+        <v>1</v>
+      </c>
+      <c r="N31" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B32" s="4"/>
+      <c r="H32" t="s">
+        <v>7</v>
+      </c>
+      <c r="I32" t="str">
+        <v>45627|45631</v>
+      </c>
+      <c r="J32" s="4" cm="1">
+        <f t="array" ref="J32:K32">_xlfn.TEXTSPLIT(I32,"|")+0</f>
+        <v>45627</v>
+      </c>
+      <c r="K32" s="4">
+        <v>45631</v>
+      </c>
+      <c r="M32" t="b">
+        <v>1</v>
+      </c>
+      <c r="N32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B33" s="4"/>
+      <c r="H33" t="s">
+        <v>8</v>
+      </c>
+      <c r="I33" t="str">
+        <v>45631|45641</v>
+      </c>
+      <c r="J33" s="4" cm="1">
+        <f t="array" ref="J33:K33">_xlfn.TEXTSPLIT(I33,"|")+0</f>
+        <v>45631</v>
+      </c>
+      <c r="K33" s="4">
+        <v>45641</v>
+      </c>
+      <c r="M33" t="b">
+        <v>1</v>
+      </c>
+      <c r="N33" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B34" s="4"/>
+      <c r="H34" t="s">
+        <v>9</v>
+      </c>
+      <c r="I34" t="str">
+        <v>45627|45635</v>
+      </c>
+      <c r="J34" s="4" cm="1">
+        <f t="array" ref="J34:K34">_xlfn.TEXTSPLIT(I34,"|")+0</f>
+        <v>45627</v>
+      </c>
+      <c r="K34" s="4">
+        <v>45635</v>
+      </c>
+      <c r="M34" t="b">
+        <v>1</v>
+      </c>
+      <c r="N34" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B35" s="4"/>
+      <c r="H35" t="s">
+        <v>10</v>
+      </c>
+      <c r="I35" t="str">
+        <v>45641|45644</v>
+      </c>
+      <c r="J35" s="4" cm="1">
+        <f t="array" ref="J35:K35">_xlfn.TEXTSPLIT(I35,"|")+0</f>
+        <v>45641</v>
+      </c>
+      <c r="K35" s="4">
+        <v>45644</v>
+      </c>
+      <c r="M35" t="b">
+        <v>1</v>
+      </c>
+      <c r="N35" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B36" s="4"/>
+      <c r="H36" t="s">
+        <v>11</v>
+      </c>
+      <c r="I36" t="str">
+        <v>45631|45638</v>
+      </c>
+      <c r="J36" s="4" cm="1">
+        <f t="array" ref="J36:K36">_xlfn.TEXTSPLIT(I36,"|")+0</f>
+        <v>45631</v>
+      </c>
+      <c r="K36" s="4">
+        <v>45638</v>
+      </c>
+      <c r="M36" t="b">
+        <v>1</v>
+      </c>
+      <c r="N36" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B37" s="4"/>
+      <c r="H37" t="s">
+        <v>12</v>
+      </c>
+      <c r="I37" t="str">
+        <v>45638|45643</v>
+      </c>
+      <c r="J37" s="4" cm="1">
+        <f t="array" ref="J37:K37">_xlfn.TEXTSPLIT(I37,"|")+0</f>
+        <v>45638</v>
+      </c>
+      <c r="K37" s="4">
+        <v>45643</v>
+      </c>
+      <c r="M37" t="b">
+        <v>1</v>
+      </c>
+      <c r="N37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B38" s="4"/>
+      <c r="H38" t="s">
+        <v>13</v>
+      </c>
+      <c r="I38" t="str">
+        <v>45638|45648</v>
+      </c>
+      <c r="J38" s="4" cm="1">
+        <f t="array" ref="J38:K38">_xlfn.TEXTSPLIT(I38,"|")+0</f>
+        <v>45638</v>
+      </c>
+      <c r="K38" s="4">
+        <v>45648</v>
+      </c>
+      <c r="M38" t="b">
+        <v>1</v>
+      </c>
+      <c r="N38" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B39" s="4"/>
+      <c r="H39" t="s">
+        <v>14</v>
+      </c>
+      <c r="I39" t="str">
+        <v>45648|45652</v>
+      </c>
+      <c r="J39" s="4" cm="1">
+        <f t="array" ref="J39:K39">_xlfn.TEXTSPLIT(I39,"|")+0</f>
+        <v>45648</v>
+      </c>
+      <c r="K39" s="4">
+        <v>45652</v>
+      </c>
+      <c r="M39" t="b">
+        <v>1</v>
+      </c>
+      <c r="N39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="H40" t="s">
+        <v>15</v>
+      </c>
+      <c r="I40" t="str">
+        <v>45652|45652</v>
+      </c>
+      <c r="J40" s="4" cm="1">
+        <f t="array" ref="J40:K40">_xlfn.TEXTSPLIT(I40,"|")+0</f>
+        <v>45652</v>
+      </c>
+      <c r="K40" s="4">
+        <v>45652</v>
+      </c>
+      <c r="M40" t="b">
+        <v>1</v>
+      </c>
+      <c r="N40" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<AFEJSONBlob xmlns="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0">ewAiAHMAYwBoAGUAbQBhACIAOgAiAGgAdAB0AHAAOgAvAC8AcwBjAGgAZQBtAGEAcwAuAGEAZAB2AGEAbgBjAGUAZABmAG8AcgBtAHUAbABhAGUAbgB2AGkAcgBvAG4AbQBlAG4AdAAuAG8AZgBmAGkAYwBlAGEAcABwAHMALgBsAGkAdgBlAC4AYwBvAG0ALwBhAGYAZQBwAHIAbwBqAGUAYwB0AHMALwAwAC4AMgAiACwAIgBmAGkAbABlAHMAIgA6AFsAewAiAHAAYQB0AGgAIgA6ACIALwBwAHIAbwBqAGUAYwB0AHMALwBXAG8AcgBrAGIAbwBvAGsAIgAsACIAdABlAHgAdAAiADoAIgAvAC8AIAAtAC0ALQAgAFcAbwByAGsAYgBvAG8AawAgAG0AbwBkAHUAbABlACAALQAtAC0AXABuAC8ALwAgAEEAIABmAGkAbABlACAAbwBmACAAbgBhAG0AZQAgAGQAZQBmAGkAbgBpAHQAaQBvAG4AcwAgAG8AZgAgAHQAaABlACAAZgBvAHIAbQA6AFwAbgAvAC8AIAAgACAAIABuAGEAbQBlACAAPQAgAGQAZQBmAGkAbgBpAHQAaQBvAG4AOwBcAG4AIgB9AF0ALAAiAHAAcgBvAGoAZQBjAHQATgBhAG0AZQBzACIAOgBbAF0ALAAiAGwAbwBjAGEAbABlACIAOgB7ACIAbABpAHMAdABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHIAbwB3AFMAZQBwAGEAcgBhAHQAbwByACIAOgAiADsAIgAsACIAYwBvAGwAdQBtAG4AUwBlAHAAYQByAGEAdABvAHIAIgA6ACIALAAiACwAIgB0AGgAbwB1AHMAYQBuAGQAcwBTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHQAaABvAHUAcwBhAG4AZABzAFAAbwBzAGkAdABpAG8AbgBzACIAOgBbADMAXQAsACIAZABlAGMAaQBtAGEAbABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAuACIALAAiAGQAYQB0AGUATwByAGQAZQByACIAOgAiAEQATQBZACIALAAiAGMAdQByAHIAZQBuAGMAeQBTAHkAbQBiAG8AbAAiADoAIgAkACIALAAiAGkAcwBDAHUAcgByAGUAbgBjAHkAUwB5AG0AYgBvAGwATABlAGEAZAAiADoAdAByAHUAZQAsACIAaQBzAEMAdQByAHIAZQBuAGMAeQBTAGUAcABCAHkAUwBwAGEAYwBlACIAOgBmAGEAbABzAGUALAAiAHIAbwB3AEwAZQB0AHQAZQByACIAOgAiAFIAIgAsACIAYwBvAGwAdQBtAG4ATABlAHQAdABlAHIAIgA6ACIAQwAiACwAIgByAGMATABlAGYAdABCAHIAYQBjAGsAZQB0ACIAOgAiAFsAIgAsACIAcgBjAFIAaQBnAGgAdABCAHIAYQBjAGsAZQB0ACIAOgAiAF0AIgAsACIAcwB0AGEAdABlAG0AZQBuAHQAUwBlAHAAYQByAGEAdABvAHIAIgA6ACIAOwAiACwAIgBsAG8AYwBhAGwAZQBOAGEAbQBlACIAOgAiAGUAbgAtAHUAcwAiAH0AfQA=</AFEJSONBlob>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EF13DA5-5E49-4A3F-B222-FEA447D244EB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>